<commit_message>
add estimations for Luke
</commit_message>
<xml_diff>
--- a/assignment-2/lj-a2-estimations.xlsx
+++ b/assignment-2/lj-a2-estimations.xlsx
@@ -384,7 +384,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -429,10 +429,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,11 +441,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,18 +581,18 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="18.6122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="76.6734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="75.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -659,7 +655,7 @@
       <c r="C4" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="D4" s="11" t="n">
+      <c r="D4" s="10" t="n">
         <v>30</v>
       </c>
       <c r="E4" s="10" t="n">
@@ -671,7 +667,7 @@
       <c r="G4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="12" t="n">
+      <c r="H4" s="11" t="n">
         <f aca="false">AVERAGEIF(B4:G4,"&gt;0")</f>
         <v>32.3333333333333</v>
       </c>
@@ -686,7 +682,7 @@
       <c r="C5" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="10" t="n">
         <v>15</v>
       </c>
       <c r="E5" s="10" t="n">
@@ -698,7 +694,7 @@
       <c r="G5" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="H5" s="12" t="n">
+      <c r="H5" s="11" t="n">
         <f aca="false">AVERAGEIF(B5:G5,"&gt;0")</f>
         <v>10.6666666666667</v>
       </c>
@@ -707,124 +703,132 @@
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="15" t="n">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13" t="n">
         <v>40</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="15" t="n">
+      <c r="D6" s="13" t="n">
+        <v>40</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13" t="n">
         <v>49</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="12" t="n">
+      <c r="G6" s="14"/>
+      <c r="H6" s="11" t="n">
         <f aca="false">AVERAGEIF(B6:G6,"&gt;0")</f>
-        <v>44.5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="15" t="n">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="D7" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="15" t="n">
+      <c r="E7" s="14"/>
+      <c r="F7" s="13" t="n">
         <v>32</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="12" t="n">
+      <c r="G7" s="14"/>
+      <c r="H7" s="11" t="n">
         <f aca="false">AVERAGEIF(B7:G7,"&gt;0")</f>
-        <v>21</v>
+        <v>19.3333333333333</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="15" t="n">
+      <c r="B8" s="12"/>
+      <c r="C8" s="15" t="n">
         <v>30</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="15" t="n">
+      <c r="D8" s="13" t="n">
+        <v>30</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="13" t="n">
         <v>32</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="12" t="n">
+      <c r="G8" s="14"/>
+      <c r="H8" s="11" t="n">
         <f aca="false">AVERAGEIF(B8:G8,"&gt;0")</f>
-        <v>31</v>
+        <v>30.6666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15" t="n">
+      <c r="B9" s="12"/>
+      <c r="C9" s="15" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" s="13" t="n">
         <v>30</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15" t="n">
+      <c r="E9" s="14"/>
+      <c r="F9" s="13" t="n">
         <v>40</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="12" t="n">
+      <c r="G9" s="14"/>
+      <c r="H9" s="11" t="n">
         <f aca="false">AVERAGEIF(B9:G9,"&gt;0")</f>
-        <v>35</v>
+        <v>31.6666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15" t="n">
+      <c r="B10" s="12"/>
+      <c r="C10" s="15" t="n">
+        <v>24</v>
+      </c>
+      <c r="D10" s="13" t="n">
         <v>25</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="15" t="n">
+      <c r="E10" s="14"/>
+      <c r="F10" s="13" t="n">
         <v>39</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="12" t="n">
+      <c r="G10" s="14"/>
+      <c r="H10" s="11" t="n">
         <f aca="false">AVERAGEIF(B10:G10,"&gt;0")</f>
-        <v>32</v>
+        <v>29.3333333333333</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15" t="n">
+      <c r="B11" s="12"/>
+      <c r="C11" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="15" t="n">
+      <c r="E11" s="14"/>
+      <c r="F11" s="13" t="n">
         <v>22</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="12" t="n">
+      <c r="G11" s="14"/>
+      <c r="H11" s="11" t="n">
         <f aca="false">AVERAGEIF(B11:G11,"&gt;0")</f>
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H12" s="17" t="n">
+      <c r="H12" s="16" t="n">
         <f aca="false">SUM(H4:H11)</f>
-        <v>222.5</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -988,536 +992,536 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="198.887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="17" width="196.683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" customFormat="false" ht="23.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="22" t="n">
+      <c r="B5" s="21" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="22" t="n">
+      <c r="B6" s="21" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="22" t="n">
+      <c r="B7" s="21" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="21" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="22" t="n">
+      <c r="B9" s="21" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="22" t="n">
+      <c r="B10" s="21" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="25" t="n">
+      <c r="B11" s="24" t="n">
         <f aca="false">SUM(B5:B10)</f>
         <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="22" t="n">
+      <c r="B15" s="21" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="22" t="n">
+      <c r="B16" s="21" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="25" t="n">
+      <c r="B17" s="24" t="n">
         <f aca="false">SUM(B15:B16)</f>
         <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="22"/>
+      <c r="B20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="22" t="n">
+      <c r="B21" s="21" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="22" t="n">
+      <c r="B22" s="21" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="22" t="n">
+      <c r="B23" s="21" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="22" t="n">
+      <c r="B24" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="22" t="n">
+      <c r="B25" s="21" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="25" t="n">
+      <c r="B26" s="24" t="n">
         <f aca="false">SUM(B21:B25)</f>
         <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9"/>
-      <c r="B27" s="22"/>
+      <c r="B27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="22"/>
+      <c r="B28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="22"/>
+      <c r="B29" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="22" t="n">
+      <c r="B30" s="21" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="22" t="n">
+      <c r="B31" s="21" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="22" t="n">
+      <c r="B32" s="21" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="22" t="n">
+      <c r="B33" s="21" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="22" t="n">
+      <c r="B34" s="21" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="22" t="n">
+      <c r="B35" s="21" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="25" t="n">
+      <c r="B36" s="24" t="n">
         <f aca="false">SUM(B30:B35)</f>
         <v>32</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9"/>
-      <c r="B37" s="22"/>
+      <c r="B37" s="21"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="22"/>
+      <c r="B38" s="21"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="22"/>
+      <c r="B39" s="21"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="22" t="n">
+      <c r="B40" s="21" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="22" t="n">
+      <c r="B41" s="21" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="22" t="n">
+      <c r="B42" s="21" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="22" t="n">
+      <c r="B43" s="21" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="22" t="n">
+      <c r="B44" s="21" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="25" t="n">
+      <c r="B45" s="24" t="n">
         <f aca="false">SUM(B40:B44)</f>
         <v>32</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9"/>
-      <c r="B46" s="22"/>
+      <c r="B46" s="21"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="22"/>
+      <c r="B47" s="21"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="22"/>
+      <c r="B48" s="21"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="22" t="n">
+      <c r="B49" s="21" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="26" t="s">
+      <c r="A50" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="22" t="n">
+      <c r="B50" s="21" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="22" t="n">
+      <c r="B51" s="21" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="26" t="s">
+      <c r="A52" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="22" t="n">
+      <c r="B52" s="21" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="22" t="n">
+      <c r="B53" s="21" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="25" t="n">
+      <c r="B54" s="24" t="n">
         <f aca="false">SUM(B49:B53)</f>
         <v>40</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9"/>
-      <c r="B55" s="22"/>
+      <c r="B55" s="21"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="22"/>
+      <c r="B56" s="21"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="22"/>
+      <c r="B57" s="21"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="22" t="n">
+      <c r="B58" s="21" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B59" s="22" t="n">
+      <c r="B59" s="21" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="26" t="s">
+      <c r="A60" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="22" t="n">
+      <c r="B60" s="21" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B61" s="22" t="n">
+      <c r="B61" s="21" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B62" s="22" t="n">
+      <c r="B62" s="21" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="26" t="s">
+      <c r="A63" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="22" t="n">
+      <c r="B63" s="21" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="25" t="n">
+      <c r="B64" s="24" t="n">
         <f aca="false">SUM(B58:B63)</f>
         <v>39</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9"/>
-      <c r="B65" s="22"/>
+      <c r="B65" s="21"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B66" s="22"/>
+      <c r="B66" s="21"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="22"/>
+      <c r="B67" s="21"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="26" t="s">
+      <c r="A68" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B68" s="22" t="n">
+      <c r="B68" s="21" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="26" t="s">
+      <c r="A69" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="22" t="n">
+      <c r="B69" s="21" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B70" s="22" t="n">
+      <c r="B70" s="21" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="26" t="s">
+      <c r="A71" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B71" s="29" t="n">
+      <c r="B71" s="28" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="26" t="s">
+      <c r="A72" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B72" s="29" t="n">
+      <c r="B72" s="28" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="24" t="s">
+      <c r="A73" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B73" s="25" t="n">
+      <c r="B73" s="24" t="n">
         <f aca="false">SUM(B68:B72)</f>
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
update estimation for backups as MLab makes this really easy
</commit_message>
<xml_diff>
--- a/assignment-2/lj-a2-estimations.xlsx
+++ b/assignment-2/lj-a2-estimations.xlsx
@@ -581,7 +581,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -810,7 +810,7 @@
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11" s="13" t="n">
         <v>10</v>
@@ -822,13 +822,13 @@
       <c r="G11" s="14"/>
       <c r="H11" s="11" t="n">
         <f aca="false">AVERAGEIF(B11:G11,"&gt;0")</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H12" s="16" t="n">
         <f aca="false">SUM(H4:H11)</f>
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>